<commit_message>
alteração na base de dados (criação do modelo)
alteração na base de dados (criação do modelo)
crição do modelo da base de dados...
</commit_message>
<xml_diff>
--- a/Estudos/diagrama_der.xlsx
+++ b/Estudos/diagrama_der.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="60" windowWidth="11415" windowHeight="5385"/>
+    <workbookView xWindow="120" yWindow="60" windowWidth="11415" windowHeight="5385" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="doc" sheetId="8" r:id="rId1"/>
@@ -379,6 +379,204 @@
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>486060</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>76739</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="3957686" cy="937629"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Retângulo 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5496210" y="2743739"/>
+          <a:ext cx="3957686" cy="937629"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr wrap="none" lIns="91440" tIns="45720" rIns="91440" bIns="45720">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="5400" b="1" cap="none" spc="0">
+              <a:ln w="12700">
+                <a:solidFill>
+                  <a:schemeClr val="tx2">
+                    <a:satMod val="155000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:solidFill>
+                <a:schemeClr val="bg2">
+                  <a:tint val="85000"/>
+                  <a:satMod val="155000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="41275" dist="20320" dir="1800000" algn="tl" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="40000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </a:rPr>
+            <a:t>ok modelado</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>2419350</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="3957686" cy="937629"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Retângulo 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3876675" y="2838450"/>
+          <a:ext cx="3957686" cy="937629"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr wrap="none" lIns="91440" tIns="45720" rIns="91440" bIns="45720">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="5400" b="1" cap="none" spc="0">
+              <a:ln w="12700">
+                <a:solidFill>
+                  <a:schemeClr val="tx2">
+                    <a:satMod val="155000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:solidFill>
+                <a:schemeClr val="bg2">
+                  <a:tint val="85000"/>
+                  <a:satMod val="155000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="41275" dist="20320" dir="1800000" algn="tl" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="40000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </a:rPr>
+            <a:t>ok modelado</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="3957686" cy="937629"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Retângulo 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3971925" y="2095500"/>
+          <a:ext cx="3957686" cy="937629"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr wrap="none" lIns="91440" tIns="45720" rIns="91440" bIns="45720">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="5400" b="1" cap="none" spc="0">
+              <a:ln w="12700">
+                <a:solidFill>
+                  <a:schemeClr val="tx2">
+                    <a:satMod val="155000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:solidFill>
+                <a:schemeClr val="bg2">
+                  <a:tint val="85000"/>
+                  <a:satMod val="155000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="41275" dist="20320" dir="1800000" algn="tl" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="40000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </a:rPr>
+            <a:t>ok modelado</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -668,8 +866,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -797,7 +995,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -848,6 +1046,7 @@
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -969,6 +1168,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -976,8 +1176,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1083,6 +1283,7 @@
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
versionamento da tela de descanso
</commit_message>
<xml_diff>
--- a/Estudos/diagrama_der.xlsx
+++ b/Estudos/diagrama_der.xlsx
@@ -995,7 +995,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1055,7 +1055,7 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1177,7 +1177,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="B7" sqref="B7:B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>